<commit_message>
august data and added reproductive column
</commit_message>
<xml_diff>
--- a/GW_seaweed_reproductive_timing.xlsx
+++ b/GW_seaweed_reproductive_timing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{45A392D3-FA9E-48FB-86B4-FFFC51A56A71}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4D87308-72AD-40DC-8FF7-E2BEB3C36D23}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,13 +379,14 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed phylum names marker and href
</commit_message>
<xml_diff>
--- a/GW_seaweed_reproductive_timing.xlsx
+++ b/GW_seaweed_reproductive_timing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD592D9C-C5D0-46F7-AC25-15AC107DC021}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B45FAC2C-511D-45A5-9A7C-77A70600135E}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>year</t>
   </si>
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,6 +477,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added dec 2022 data from dev branch
</commit_message>
<xml_diff>
--- a/GW_seaweed_reproductive_timing.xlsx
+++ b/GW_seaweed_reproductive_timing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B45FAC2C-511D-45A5-9A7C-77A70600135E}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_F25DC773A252ABDACC104848C1586FFC5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B3BB811-C9A7-4A62-9EB2-142A7571F3BF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>year</t>
   </si>
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,6 +491,34 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2022</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2023</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>